<commit_message>
Scripting SCD0331 until SCD0333
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0331 - Normal Skenario Menjalankan Fungsi scheduler ConsoleBlastNotifSalesLogin.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0331 - Normal Skenario Menjalankan Fungsi scheduler ConsoleBlastNotifSalesLogin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2AB338-5C4E-4316-BF85-8C67C60397B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BEAB87-232C-4E7F-947B-63A395AA513E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>FILE1</t>
   </si>
   <si>
-    <t>DGS-347</t>
-  </si>
-  <si>
     <t>Normal Skenario Menjalankan Fungsi scheduler ConsoleBlastNotifSalesLogin</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>Report Log WA</t>
+  </si>
+  <si>
+    <t>DGS-346</t>
   </si>
 </sst>
 </file>
@@ -542,7 +542,7 @@
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,16 +620,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>16</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>17</v>
       </c>
       <c r="F2" s="17">
         <v>52326</v>
@@ -638,22 +638,22 @@
         <v>9</v>
       </c>
       <c r="H2" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>18</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>19</v>
       </c>
       <c r="J2" s="14"/>
       <c r="K2" s="14"/>
       <c r="L2" s="17" t="str">
         <f ca="1">TEXT(TODAY(),"yyyy/mm/dd") &amp;" - "&amp; TEXT(TODAY(),"yyyy/mm/dd")</f>
-        <v>2022/09/12 - 2022/09/12</v>
+        <v>2022/09/13 - 2022/09/13</v>
       </c>
       <c r="M2" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="14" t="s">
         <v>21</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>22</v>
       </c>
       <c r="O2" s="14"/>
       <c r="P2" s="14"/>

</xml_diff>